<commit_message>
1. Source file indexing logic improved for AspectJ 2. Regular expression for parsing stackTrace was improved.
</commit_message>
<xml_diff>
--- a/doc/Development status.xlsx
+++ b/doc/Development status.xlsx
@@ -217,10 +217,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>mm"월"\ dd"일"</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42019</c:v>
                 </c:pt>
@@ -232,16 +232,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>11</c:v>
                 </c:pt>
@@ -252,6 +255,9 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
@@ -287,10 +293,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>mm"월"\ dd"일"</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42019</c:v>
                 </c:pt>
@@ -302,16 +308,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>51</c:v>
                 </c:pt>
@@ -323,6 +332,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,11 +350,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="287694448"/>
-        <c:axId val="287695568"/>
+        <c:axId val="196222960"/>
+        <c:axId val="196228000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="287694448"/>
+        <c:axId val="196222960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,7 +397,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287695568"/>
+        <c:crossAx val="196228000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -393,7 +405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="287695568"/>
+        <c:axId val="196228000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +513,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="287694448"/>
+        <c:crossAx val="196222960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -698,10 +710,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>mm"월"\ dd"일"</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42019</c:v>
                 </c:pt>
@@ -713,16 +725,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$5</c:f>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>3062</c:v>
                 </c:pt>
@@ -734,6 +749,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,10 +786,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>mm"월"\ dd"일"</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42019</c:v>
                 </c:pt>
@@ -783,16 +801,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42047</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$5</c:f>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4577</c:v>
                 </c:pt>
@@ -804,6 +825,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8653</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,11 +843,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="337410512"/>
-        <c:axId val="309896368"/>
+        <c:axId val="248179872"/>
+        <c:axId val="194221040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="337410512"/>
+        <c:axId val="248179872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +890,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309896368"/>
+        <c:crossAx val="194221040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -874,7 +898,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309896368"/>
+        <c:axId val="194221040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +1006,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="337410512"/>
+        <c:crossAx val="248179872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2186,16 +2210,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2216,16 +2240,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>633412</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2510,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2607,6 +2631,23 @@
         <v>8653</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>42076</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>89</v>
+      </c>
+      <c r="D6">
+        <v>7188</v>
+      </c>
+      <c r="E6">
+        <v>10377</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>